<commit_message>
First two sheets working?
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -15,21 +15,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+  <si>
+    <t>Business Transaction Name</t>
+  </si>
+  <si>
+    <t>Transaction Description</t>
+  </si>
+  <si>
+    <t>Business Volumes</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
   <si>
     <t>Business Transaction</t>
   </si>
   <si>
-    <t>Transaction Description</t>
-  </si>
-  <si>
-    <t>Business Volumes</t>
-  </si>
-  <si>
-    <t>Frequency</t>
-  </si>
-  <si>
-    <t>Notes</t>
+    <t>IT Transaction Name</t>
+  </si>
+  <si>
+    <t>IT Transaction Description</t>
+  </si>
+  <si>
+    <t>Qty per transaction</t>
+  </si>
+  <si>
+    <t>Transaction Rating</t>
+  </si>
+  <si>
+    <t>TPS</t>
   </si>
   <si>
     <t>Process Enquiry</t>
@@ -38,30 +56,65 @@
     <t>Process Enquiry / Application</t>
   </si>
   <si>
+    <t>80</t>
+  </si>
+  <si>
     <t>per hour</t>
   </si>
   <si>
-    <t>IT Transaction Name</t>
-  </si>
-  <si>
-    <t>IT Transaction Description</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Transaction Rating</t>
-  </si>
-  <si>
-    <t>TPS</t>
+    <t>Contact NRP and Gather Information</t>
+  </si>
+  <si>
+    <t>Shared Care Resolution</t>
+  </si>
+  <si>
+    <t>Transition</t>
+  </si>
+  <si>
+    <t>Transition Existing Scheme</t>
+  </si>
+  <si>
+    <t>Financial Transition</t>
+  </si>
+  <si>
+    <t>Reactive Transition</t>
+  </si>
+  <si>
+    <t>Manage Reactive Transition to Future Scheme</t>
+  </si>
+  <si>
+    <t>Deetermine Parentage</t>
+  </si>
+  <si>
+    <t>Determine Parentage</t>
+  </si>
+  <si>
+    <t>Manage Client Contact</t>
+  </si>
+  <si>
+    <t>Perform Calculation</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>This needs to be checked</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -89,8 +142,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,41 +439,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A7:E8"/>
+  <dimension ref="A7:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>80</v>
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -429,42 +524,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A7:F8"/>
+  <dimension ref="A7:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <f>'Input Business Transactions'!A8</f>
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -473,7 +571,86 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <f>'Input Business Transactions'!C8</f>
+        <f>'Input Business Transactions'!C8*D8*E8/60/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <f>'Input Business Transactions'!A8</f>
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f>'Input Business Transactions'!C8*D9*E9/60/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <f>'Input Business Transactions'!A8</f>
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>0.0875</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <f>'Input Business Transactions'!C8*D10*E10/60/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <f>'Input Business Transactions'!A9</f>
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f>'Input Business Transactions'!C9*D11*E11/60/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <f>'Input Business Transactions'!A9</f>
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f>'Input Business Transactions'!C9*D12*E12/60/60</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>